<commit_message>
product of array except self added.
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ma/Desktop/Projects/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99CC135-1811-1246-BE4C-3EF88BB5321F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8147871E-3131-F642-8BD6-AC302C375F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1556,7 +1556,7 @@
   <dimension ref="A1:F1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1565,7 +1565,7 @@
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
     <col min="3" max="3" width="64" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.5" customWidth="1"/>
     <col min="6" max="6" width="146.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
new code added to MaximimProductSubarray
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ma/Desktop/Projects/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A375D0-457C-784C-AC63-6FC5D35FF8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B01D8A-F3D8-D143-89DB-A9161AA5D549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="320">
   <si>
     <t>A BETTER VERSION -&gt;&gt;</t>
   </si>
@@ -983,9 +983,6 @@
   </si>
   <si>
     <t>✅</t>
-  </si>
-  <si>
-    <t>💩</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1362,9 +1359,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1589,7 +1583,7 @@
   <dimension ref="A1:F1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1709,10 +1703,10 @@
       <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="29" t="s">
         <v>319</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -1733,7 +1727,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>26</v>
@@ -1752,7 +1746,9 @@
       <c r="C9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="29"/>
+      <c r="D9" s="29" t="s">
+        <v>319</v>
+      </c>
       <c r="E9" s="11" t="s">
         <v>30</v>
       </c>
@@ -5806,145 +5802,145 @@
     <hyperlink ref="A9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="A10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="A11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E11" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="A12" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="A13" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E13" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A14" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E14" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A15" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E15" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A16" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E16" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A17" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E17" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A18" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="E18" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A19" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="E19" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="A20" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="E20" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A21" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="E21" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="A22" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="E22" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A23" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="E23" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="A24" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="E24" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="A25" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="E25" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="A26" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="E26" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="A27" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="E27" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="A28" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="E28" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="A29" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="E29" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="A30" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="E30" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="A31" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="E31" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="A32" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="E32" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="A33" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="E33" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="A34" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="E34" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="A35" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="E35" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="A36" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="E36" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="A37" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="E37" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="A38" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="E38" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="A39" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="E39" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="A40" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="E40" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="A41" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="E41" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="A42" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="E42" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="A43" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="E43" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="A44" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="E44" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="A45" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="E45" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="A46" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="E46" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="A47" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="E47" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="A48" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="E48" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="A49" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="E49" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="A50" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="E50" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="A51" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="E51" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="A52" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="E52" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="A53" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="E53" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="A54" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="E54" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="A55" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="E55" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="A56" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="E56" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="A57" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="E57" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="A58" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="E58" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="A59" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="E59" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="A60" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="E60" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="A61" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="E61" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="A62" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="E62" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="A63" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="E63" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="A64" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="E64" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="A65" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="E65" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="A66" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="E66" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="A67" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="E67" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="A68" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="E68" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="A69" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="E69" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="A70" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="E70" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="A71" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="E71" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="A72" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="E72" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="A73" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="E73" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="A74" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="E74" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="A75" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="E75" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="A76" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="E76" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="A77" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="E77" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="A78" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="E78" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="A79" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="E79" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="A11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A12" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E12" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A13" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E13" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A14" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E14" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A15" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E15" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A16" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E16" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A17" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E17" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A18" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E18" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A19" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E19" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A20" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E20" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A21" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E21" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A22" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E22" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="A23" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E23" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="A24" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E24" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="A25" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E25" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A26" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E26" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A27" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E27" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="A28" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E28" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A29" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="E29" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="A30" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="E30" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="A31" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="E31" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="A32" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="E32" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="A33" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="E33" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="A34" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="E34" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="A35" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="E35" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="A36" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="E36" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="A37" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="E37" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="A38" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="E38" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="A39" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="E39" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="A40" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="E40" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="A41" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="E41" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A42" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="E42" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="A43" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="E43" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="A44" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="E44" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="A45" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="E45" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="A46" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="E46" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A47" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="E47" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="A48" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="E48" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="A49" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E49" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="A50" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E50" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="A51" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="E51" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="A52" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="E52" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="A53" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="E53" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="A54" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="E54" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="A55" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="E55" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="A56" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="E56" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="A57" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="E57" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="A58" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="E58" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="A59" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="E59" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="A60" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="E60" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="A61" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="E61" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="A62" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="E62" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="A63" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="E63" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="A64" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="E64" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="A65" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="E65" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="A66" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="E66" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="A67" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="E67" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="A68" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="E68" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="A69" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="E69" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="A70" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="E70" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="A71" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="E71" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="A72" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="E72" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="A73" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="E73" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="A74" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="E74" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="A75" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="E75" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="A76" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="E76" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="A77" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="E77" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="A78" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="E78" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="A79" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="E79" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="E10" r:id="rId153" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some codes are updated.
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ma/Desktop/Projects/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B01D8A-F3D8-D143-89DB-A9161AA5D549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C94762-3BDA-984B-8C1B-F182566BFDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="320">
   <si>
     <t>A BETTER VERSION -&gt;&gt;</t>
   </si>
@@ -1583,7 +1583,7 @@
   <dimension ref="A1:F1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1766,7 +1766,9 @@
       <c r="C10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="29"/>
+      <c r="D10" s="29" t="s">
+        <v>319</v>
+      </c>
       <c r="E10" s="11" t="s">
         <v>34</v>
       </c>

</xml_diff>